<commit_message>
Updated the data field
</commit_message>
<xml_diff>
--- a/ta-scheduler-timefold/data/availability_Template.xlsx
+++ b/ta-scheduler-timefold/data/availability_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danialnoorizadeh/Code/ShiftScheduler/ta-scheduler-ortools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danialnoorizadeh/Code/ShiftScheduler/ta-scheduler-timefold/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558A1CBC-0990-FD43-AAA9-75BF6ED92A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0577E070-2EB8-064E-86AC-F3D34967B79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="500" windowWidth="21800" windowHeight="13920" xr2:uid="{98118C80-EDF3-C141-9DFA-EEAB9BD2538B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{98118C80-EDF3-C141-9DFA-EEAB9BD2538B}"/>
   </bookViews>
   <sheets>
     <sheet name="availability" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Day of Week</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Availability</t>
+  </si>
+  <si>
+    <t>Instructions</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -634,6 +637,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1167,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7524CAAE-3254-7D4F-9044-EAFD77209B63}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H3" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,19 +1190,35 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="3"/>
+      <c r="H1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1201,13 +1226,36 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1223,8 +1271,15 @@
       <c r="E6" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -1240,8 +1295,15 @@
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1257,8 +1319,15 @@
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -1274,8 +1343,15 @@
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -1289,8 +1365,15 @@
         <v>20</v>
       </c>
       <c r="E10" s="1"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -1305,7 +1388,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>6</v>
       </c>
@@ -1320,7 +1403,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>7</v>
       </c>
@@ -1335,7 +1418,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -1350,7 +1433,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -1365,7 +1448,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>10</v>
       </c>
@@ -1383,6 +1466,17 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:N10"/>
+    <mergeCell ref="H1:N2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:N4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:N6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:N8"/>
+  </mergeCells>
   <conditionalFormatting sqref="E7:E16">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unavailable"</formula>

</xml_diff>